<commit_message>
Update flashmessage and export excel
</commit_message>
<xml_diff>
--- a/excel_with_dropdown.xlsx
+++ b/excel_with_dropdown.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>ID Alternatif</t>
   </si>
@@ -36,54 +36,6 @@
   </si>
   <si>
     <t>cek</t>
-  </si>
-  <si>
-    <t>95-100</t>
-  </si>
-  <si>
-    <t>90-94,99</t>
-  </si>
-  <si>
-    <t>85-89,99</t>
-  </si>
-  <si>
-    <t>&lt;=84,99</t>
-  </si>
-  <si>
-    <t>sangat baik</t>
-  </si>
-  <si>
-    <t>baik</t>
-  </si>
-  <si>
-    <t>cukup baik</t>
-  </si>
-  <si>
-    <t>kurang baik</t>
-  </si>
-  <si>
-    <t>selalu hadir</t>
-  </si>
-  <si>
-    <t>cukup hadir</t>
-  </si>
-  <si>
-    <t>jarang hadir</t>
-  </si>
-  <si>
-    <t>izin</t>
-  </si>
-  <si>
-    <t>sangat aktif</t>
-  </si>
-  <si>
-    <t>aktif</t>
-  </si>
-  <si>
-    <t>cukup aktif</t>
-  </si>
-  <si>
-    <t>kurang aktif</t>
   </si>
 </sst>
 </file>
@@ -423,7 +375,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,116 +395,49 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
+    <row r="2" spans="1:6">
+      <c r="A2">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="C19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="C20" t="s">
-        <v>22</v>
-      </c>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
     </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" errorStyle="stop" operator="between" allowBlank="0" showDropDown="0" showInputMessage="0" showErrorMessage="0" errorTitle="Input error" error="Please select a value from the list." promptTitle="Pick from list" prompt="Please pick a value from the dropdown list." sqref="C2">
+      <formula1>"95-100,90-94,85-89,&lt;=84"</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="stop" operator="between" allowBlank="0" showDropDown="0" showInputMessage="0" showErrorMessage="0" errorTitle="Input error" error="Please select a value from the list." promptTitle="Pick from list" prompt="Please pick a value from the dropdown list." sqref="D2">
+      <formula1>"sangat baik,baik,cukup baik,kurang baik"</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="stop" operator="between" allowBlank="0" showDropDown="0" showInputMessage="0" showErrorMessage="0" errorTitle="Input error" error="Please select a value from the list." promptTitle="Pick from list" prompt="Please pick a value from the dropdown list." sqref="E2">
+      <formula1>"selalu hadir,cukup hadir,jarang hadir,izin"</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="stop" operator="between" allowBlank="0" showDropDown="0" showInputMessage="0" showErrorMessage="0" errorTitle="Input error" error="Please select a value from the list." promptTitle="Pick from list" prompt="Please pick a value from the dropdown list." sqref="F2">
+      <formula1>"sangat aktif,aktif,cukup aktif,kurang aktif"</formula1>
+    </dataValidation>
+  </dataValidations>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>